<commit_message>
update heur. for v2; start v3
</commit_message>
<xml_diff>
--- a/Time_Windows.xlsx
+++ b/Time_Windows.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinghongmiao/Code/mvt-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6770EA8D-CC29-AA4E-A6DE-C936FF618830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75D556C-B134-594F-9818-ABAB639D7356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="-24520" windowWidth="30240" windowHeight="22940" activeTab="1" xr2:uid="{80C050B1-FB2F-EF4E-8D88-071846B14504}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{80C050B1-FB2F-EF4E-8D88-071846B14504}"/>
   </bookViews>
   <sheets>
     <sheet name="Even" sheetId="1" r:id="rId1"/>
-    <sheet name="StronglySkewed" sheetId="3" r:id="rId2"/>
-    <sheet name="FrontLoaded" sheetId="4" r:id="rId3"/>
-    <sheet name="Randomish" sheetId="5" r:id="rId4"/>
+    <sheet name="Skewed1" sheetId="3" r:id="rId2"/>
+    <sheet name="Skewed2" sheetId="4" r:id="rId3"/>
+    <sheet name="Randomish1" sheetId="5" r:id="rId4"/>
     <sheet name="Randomish2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2293,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB61F24E-6460-2F41-BE0D-F9BF459AF97B}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="82" workbookViewId="0">
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
@@ -4115,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64564EBB-0CEA-4D48-8745-3FDFDB45A080}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="A28" zoomScale="84" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5938,7 +5937,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView zoomScale="63" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7756,8 +7755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCF9B05-51DE-F54A-A467-D0B7589554AA}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="L68" sqref="L68"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9572,18 +9571,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEF0B03-64C7-AB4B-98FF-5868F71926E5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>